<commit_message>
Ajout de la page historique & préparation de la release 3.1.1 (#79)
* changes page & prepare release 3.1.1

* update publication request

* update workflows

* update changes page

* update changes

* Add compliance update for search flows in 3.1.1

Added compliance updates for search flows with MHD.

* Update changes.md 722d83ae04534177d6dd5bba9ae90994dbacadd4
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.1.0</t>
+    <t>3.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-14T15:43:32+00:00</t>
+    <t>2026-01-14T15:54:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>